<commit_message>
Added some student features to the datasets
</commit_message>
<xml_diff>
--- a/Info and data/Features and meanings.xlsx
+++ b/Info and data/Features and meanings.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\GitHub\Applied-Statistics-Project\Info and data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45276E1-779A-455C-A86C-FB036FB7B5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC65048D-34E5-4973-ACA6-925454F08E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{3DA52822-CFDA-408E-B1C3-39FC0A4F79A9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Features and meanings" sheetId="1" r:id="rId1"/>
+    <sheet name="Student features and meanings" sheetId="1" r:id="rId1"/>
+    <sheet name="School features and meanings" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Features and meanings'!$A$1:$E$1119</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Student features and meanings'!$A$1:$E$1119</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2457" uniqueCount="2227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2857" uniqueCount="2596">
   <si>
     <t>CNTRYID</t>
   </si>
@@ -6719,6 +6720,1113 @@
   </si>
   <si>
     <t>Status (x=used, y=potential)</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>LANGTEST</t>
+  </si>
+  <si>
+    <t>Language of Questionnaire/Assessment</t>
+  </si>
+  <si>
+    <t>SC001Q01TA</t>
+  </si>
+  <si>
+    <t>Which of the following definitions best describes the community in which your school is located?</t>
+  </si>
+  <si>
+    <t>SC013Q01TA</t>
+  </si>
+  <si>
+    <t>Is your school a public or a private school?</t>
+  </si>
+  <si>
+    <t>SC016Q01TA</t>
+  </si>
+  <si>
+    <t>Percentage of total funding for school year from: Government</t>
+  </si>
+  <si>
+    <t>SC016Q02TA</t>
+  </si>
+  <si>
+    <t>Percentage of total funding for school year from: Student fees or school charges paid by parents</t>
+  </si>
+  <si>
+    <t>SC016Q03TA</t>
+  </si>
+  <si>
+    <t>Percentage of total funding for school year from: Benefactors, donations, bequests, sponsorships, parent fundraising</t>
+  </si>
+  <si>
+    <t>SC016Q04TA</t>
+  </si>
+  <si>
+    <t>Percentage of total funding for school year from: Other</t>
+  </si>
+  <si>
+    <t>SC017Q01NA</t>
+  </si>
+  <si>
+    <t>School's instruction hindered by: A lack of teaching staff.</t>
+  </si>
+  <si>
+    <t>SC017Q02NA</t>
+  </si>
+  <si>
+    <t>School's instruction hindered by: Inadequate or poorly qualified teaching staff.</t>
+  </si>
+  <si>
+    <t>SC017Q03NA</t>
+  </si>
+  <si>
+    <t>School's instruction hindered by: A lack of assisting staff.</t>
+  </si>
+  <si>
+    <t>SC017Q04NA</t>
+  </si>
+  <si>
+    <t>School's instruction hindered by: Inadequate or poorly qualified assisting staff.</t>
+  </si>
+  <si>
+    <t>SC017Q05NA</t>
+  </si>
+  <si>
+    <t>School's instruction hindered by: A lack of educational material [...]</t>
+  </si>
+  <si>
+    <t>SC017Q06NA</t>
+  </si>
+  <si>
+    <t>School's instruction hindered by: Inadequate or poor quality educational material [...]</t>
+  </si>
+  <si>
+    <t>SC017Q07NA</t>
+  </si>
+  <si>
+    <t>School's instruction hindered by: A lack of physical infrastructure [...]</t>
+  </si>
+  <si>
+    <t>SC017Q08NA</t>
+  </si>
+  <si>
+    <t>School's instruction hindered by: Inadequate or poor quality physical infrastructure [...]</t>
+  </si>
+  <si>
+    <t>SC161Q01SA</t>
+  </si>
+  <si>
+    <t>Main responsibility for career guidance at school: Not applicable, career guidance is not available in this school</t>
+  </si>
+  <si>
+    <t>SC161Q02SA</t>
+  </si>
+  <si>
+    <t>Main responsibility for career guidance at school: All teachers share the responsibility for career guidance</t>
+  </si>
+  <si>
+    <t>SC161Q03SA</t>
+  </si>
+  <si>
+    <t>Main responsibility for career guidance at school: Specific teachers have the main responsibility for career guidance</t>
+  </si>
+  <si>
+    <t>SC161Q04SA</t>
+  </si>
+  <si>
+    <t>Main responsibility for career guidance at school: We have [...] career guidance counsellors employed at school</t>
+  </si>
+  <si>
+    <t>SC161Q05SA</t>
+  </si>
+  <si>
+    <t>Main responsibility for career guidance at school: We have [...] career guidance counsellors who regularly visit [...]</t>
+  </si>
+  <si>
+    <t>SC162Q01SA</t>
+  </si>
+  <si>
+    <t>If career guidance is available at your school, which of the statements below best describes the situation for [...]</t>
+  </si>
+  <si>
+    <t>SC155Q01HA</t>
+  </si>
+  <si>
+    <t>School's capacity using digital devices: The number of digital devices connected to the Internet is sufficient</t>
+  </si>
+  <si>
+    <t>SC155Q02HA</t>
+  </si>
+  <si>
+    <t>School's capacity using digital devices: The school's Internet bandwidth or speed is sufficient</t>
+  </si>
+  <si>
+    <t>SC155Q03HA</t>
+  </si>
+  <si>
+    <t>School's capacity using digital devices: The number of digital devices for instruction is sufficient</t>
+  </si>
+  <si>
+    <t>SC155Q04HA</t>
+  </si>
+  <si>
+    <t>School's capacity using digital devices: Digital devices [...] are sufficiently powerful in terms of computing capacity</t>
+  </si>
+  <si>
+    <t>SC155Q05HA</t>
+  </si>
+  <si>
+    <t>School's capacity using digital devices: The availability of adequate software is sufficient</t>
+  </si>
+  <si>
+    <t>SC155Q06HA</t>
+  </si>
+  <si>
+    <t>School's capacity using digital devices: Teachers have the [...] skills to integrate digital devices in instruction</t>
+  </si>
+  <si>
+    <t>SC155Q07HA</t>
+  </si>
+  <si>
+    <t>School's capacity using digital devices: Teachers have sufficient time to prepare lessons integrating digital devices</t>
+  </si>
+  <si>
+    <t>SC155Q08HA</t>
+  </si>
+  <si>
+    <t>School's capacity using digital devices: Effective professional resources for teachers to learn how to use digital [...]</t>
+  </si>
+  <si>
+    <t>SC155Q09HA</t>
+  </si>
+  <si>
+    <t>School's capacity using digital devices: An effective online learning support platform is available</t>
+  </si>
+  <si>
+    <t>SC155Q10HA</t>
+  </si>
+  <si>
+    <t>School's capacity using digital devices: Teachers are provided with incentives to integrate digital devices in [...]</t>
+  </si>
+  <si>
+    <t>SC155Q11HA</t>
+  </si>
+  <si>
+    <t>School's capacity using digital devices: The school has sufficient qualified technical assistant staff</t>
+  </si>
+  <si>
+    <t>SC156Q01HA</t>
+  </si>
+  <si>
+    <t>At school: Its own written statement about the use of digital devices</t>
+  </si>
+  <si>
+    <t>SC156Q02HA</t>
+  </si>
+  <si>
+    <t>At school: Its own written statement specifically about the use of digital devices for pedagogical purposes</t>
+  </si>
+  <si>
+    <t>SC156Q03HA</t>
+  </si>
+  <si>
+    <t>At school: A programme to use digital devices for teaching and learning in specific subjects</t>
+  </si>
+  <si>
+    <t>SC156Q04HA</t>
+  </si>
+  <si>
+    <t>At school: Regular discussions with teaching staff about the use of digital devices for pedagogical purposes</t>
+  </si>
+  <si>
+    <t>SC156Q05HA</t>
+  </si>
+  <si>
+    <t>At school: A specific programme to prepare students for responsible Internet behaviour</t>
+  </si>
+  <si>
+    <t>SC156Q06HA</t>
+  </si>
+  <si>
+    <t>At school: A specific policy about using Social Networks (&lt;Facebook&gt;, etc.) in teaching and learning</t>
+  </si>
+  <si>
+    <t>SC156Q07HA</t>
+  </si>
+  <si>
+    <t>At school: A specific programme to promote collaboration on the use of digital devices among teachers</t>
+  </si>
+  <si>
+    <t>SC156Q08HA</t>
+  </si>
+  <si>
+    <t>At school: Scheduled time for teachers to meet to share, evaluate or develop instructional materials and [...]</t>
+  </si>
+  <si>
+    <t>SC011Q01TA</t>
+  </si>
+  <si>
+    <t>SC012Q01TA</t>
+  </si>
+  <si>
+    <t>Student admission to school: Student's record of academic performance (including placement tests)</t>
+  </si>
+  <si>
+    <t>SC012Q02TA</t>
+  </si>
+  <si>
+    <t>Student admission to school: Recommendation of feeder schools</t>
+  </si>
+  <si>
+    <t>SC012Q03TA</t>
+  </si>
+  <si>
+    <t>Student admission to school: Parents' endorsement of the instructional or religious philosophy of the school</t>
+  </si>
+  <si>
+    <t>SC012Q04TA</t>
+  </si>
+  <si>
+    <t>Student admission to school: Whether the student requires or is interested in a special programme</t>
+  </si>
+  <si>
+    <t>SC012Q05TA</t>
+  </si>
+  <si>
+    <t>Student admission to school: Preference given to family members of current or former students</t>
+  </si>
+  <si>
+    <t>SC012Q06TA</t>
+  </si>
+  <si>
+    <t>Student admission to school: Residence in a particular area</t>
+  </si>
+  <si>
+    <t>SC012Q07TA</t>
+  </si>
+  <si>
+    <t>Student admission to school: Other</t>
+  </si>
+  <si>
+    <t>SC042Q01TA</t>
+  </si>
+  <si>
+    <t>School's policy for &lt;national modal grade for 15-year-olds&gt;: Students are grouped by ability into different classes.</t>
+  </si>
+  <si>
+    <t>SC042Q02TA</t>
+  </si>
+  <si>
+    <t>School's policy for &lt;national modal grade for 15-year-olds&gt;: Students are grouped by ability within their classes.</t>
+  </si>
+  <si>
+    <t>SC154Q01HA</t>
+  </si>
+  <si>
+    <t>School's use of assessments of students: To guide students' learning</t>
+  </si>
+  <si>
+    <t>SC154Q02WA</t>
+  </si>
+  <si>
+    <t>School's use of assessments of students: To inform parents about their child's progress</t>
+  </si>
+  <si>
+    <t>SC154Q03WA</t>
+  </si>
+  <si>
+    <t>School's use of assessments of students: To make decisions about students' retention or promotion</t>
+  </si>
+  <si>
+    <t>SC154Q04WA</t>
+  </si>
+  <si>
+    <t>School's use of assessments of students: To group students for instructional purposes</t>
+  </si>
+  <si>
+    <t>SC154Q05WA</t>
+  </si>
+  <si>
+    <t>School's use of assessments of students: To compare the school to &lt;district or national&gt; performance</t>
+  </si>
+  <si>
+    <t>SC154Q06WA</t>
+  </si>
+  <si>
+    <t>School's use of assessments of students: To monitor the schools progress from year to year</t>
+  </si>
+  <si>
+    <t>SC154Q07WA</t>
+  </si>
+  <si>
+    <t>School's use of assessments of students: To make judgements about teachers' effectiveness</t>
+  </si>
+  <si>
+    <t>SC154Q08WA</t>
+  </si>
+  <si>
+    <t>School's use of assessments of students: To identify aspects of instruction or the curriculum that could be improved</t>
+  </si>
+  <si>
+    <t>SC154Q09HA</t>
+  </si>
+  <si>
+    <t>School's use of assessments of students: To adapt teaching to the students' needs</t>
+  </si>
+  <si>
+    <t>SC154Q10WA</t>
+  </si>
+  <si>
+    <t>School's use of assessments of students: To compare the school with other schools</t>
+  </si>
+  <si>
+    <t>SC154Q11HA</t>
+  </si>
+  <si>
+    <t>School's use of assessments of students: To award certificates to students</t>
+  </si>
+  <si>
+    <t>SC036Q01TA</t>
+  </si>
+  <si>
+    <t>Use of achievement data in school: Achievement data are posted publicly (e.g. in the media)</t>
+  </si>
+  <si>
+    <t>SC036Q02TA</t>
+  </si>
+  <si>
+    <t>Use of achievement data in school: Achievement data are tracked over time by an administrative authority</t>
+  </si>
+  <si>
+    <t>SC036Q03NA</t>
+  </si>
+  <si>
+    <t>Use of achievement data in school: Achievement data are provided directly to parents</t>
+  </si>
+  <si>
+    <t>SC037Q01TA</t>
+  </si>
+  <si>
+    <t>Quality assurance at school: Internal evaluation/Self-evaluation</t>
+  </si>
+  <si>
+    <t>SC037Q02TA</t>
+  </si>
+  <si>
+    <t>Quality assurance at school: External evaluation</t>
+  </si>
+  <si>
+    <t>SC037Q03TA</t>
+  </si>
+  <si>
+    <t>Quality assurance at school: Written specification of the school's curricular profile and educational goals</t>
+  </si>
+  <si>
+    <t>SC037Q04TA</t>
+  </si>
+  <si>
+    <t>Quality assurance at school: Written specification of student performance standards</t>
+  </si>
+  <si>
+    <t>SC037Q05NA</t>
+  </si>
+  <si>
+    <t>Quality assurance at school: Systematic recording of data such as [...] attendance and professional development</t>
+  </si>
+  <si>
+    <t>SC037Q06NA</t>
+  </si>
+  <si>
+    <t>Quality assurance at school: Systematic recording of student test results and graduation rates</t>
+  </si>
+  <si>
+    <t>SC037Q07TA</t>
+  </si>
+  <si>
+    <t>Quality assurance at school: Seeking written feedback from students (e.g. regarding lessons, teachers or resources)</t>
+  </si>
+  <si>
+    <t>SC037Q08TA</t>
+  </si>
+  <si>
+    <t>Quality assurance at school: Teacher mentoring</t>
+  </si>
+  <si>
+    <t>SC037Q09TA</t>
+  </si>
+  <si>
+    <t>Quality assurance at school: Regular consultation aimed at school improvement [...] over a period of at least six months</t>
+  </si>
+  <si>
+    <t>SC037Q10NA</t>
+  </si>
+  <si>
+    <t>Quality assurance at school: Implementation of a standardised policy for reading subjects [...]</t>
+  </si>
+  <si>
+    <t>SC165Q01HA</t>
+  </si>
+  <si>
+    <t>Teachers' practices: [...] students learn about the histories of diverse cultural groups that live in &lt;country of test&gt;.</t>
+  </si>
+  <si>
+    <t>SC165Q02HA</t>
+  </si>
+  <si>
+    <t>Teachers' practices: [...] students learn about the histories of diverse cultural groups that live in other countries.</t>
+  </si>
+  <si>
+    <t>SC165Q03HA</t>
+  </si>
+  <si>
+    <t>Teachers' practices: [...] students learn about the cultures [...] of [...] groups that live in &lt;country of test&gt;</t>
+  </si>
+  <si>
+    <t>SC165Q04HA</t>
+  </si>
+  <si>
+    <t>Teachers' practices: [...] students learn about different cultural perspectives on historical and social events.</t>
+  </si>
+  <si>
+    <t>SC165Q05HA</t>
+  </si>
+  <si>
+    <t>Teachers' practices: Our school supports activities that encourage students expression of diverse identities [...]</t>
+  </si>
+  <si>
+    <t>SC165Q06HA</t>
+  </si>
+  <si>
+    <t>Teachers' practices: Our school offers an exchange programme with schools in other countries.</t>
+  </si>
+  <si>
+    <t>SC165Q07HA</t>
+  </si>
+  <si>
+    <t>Teachers' practices: Our school organises multicultural events (e.g. cultural diversity day).</t>
+  </si>
+  <si>
+    <t>SC165Q08HA</t>
+  </si>
+  <si>
+    <t>Teachers' practices: In our school, we celebrate festivities from other cultures.</t>
+  </si>
+  <si>
+    <t>SC165Q09HA</t>
+  </si>
+  <si>
+    <t>Teachers' practices: In our school, students are encouraged to communicate with people from other cultures via [...]</t>
+  </si>
+  <si>
+    <t>SC165Q10HA</t>
+  </si>
+  <si>
+    <t>Teachers' practices: Our school adopts different approaches to educate students about cultural differences [...]</t>
+  </si>
+  <si>
+    <t>SC166Q02HA</t>
+  </si>
+  <si>
+    <t>Opinion shared by teaching staff: It is important for students to learn that people from other cultures can have [...]</t>
+  </si>
+  <si>
+    <t>SC166Q03HA</t>
+  </si>
+  <si>
+    <t>Opinion shared by teaching staff: Respecting other cultures is something that students should learn as early as possible</t>
+  </si>
+  <si>
+    <t>SC166Q05HA</t>
+  </si>
+  <si>
+    <t>Opinion shared by teaching staff: In the classroom, it is important that students of different origins recognise [...]</t>
+  </si>
+  <si>
+    <t>SC166Q06HA</t>
+  </si>
+  <si>
+    <t>Opinion shared by teaching staff: When there are conflicts between students of different origins, they should be [...]</t>
+  </si>
+  <si>
+    <t>SC167Q01HA</t>
+  </si>
+  <si>
+    <t>Curriculum for the following in &lt;national modal grade for 15-year-olds&gt;: Communicating with people from different [...]</t>
+  </si>
+  <si>
+    <t>SC167Q02HA</t>
+  </si>
+  <si>
+    <t>Curriculum for the following in &lt;national modal grade for 15-year-olds&gt;: Knowledge of different cultures</t>
+  </si>
+  <si>
+    <t>SC167Q03HA</t>
+  </si>
+  <si>
+    <t>Curriculum for the following in &lt;national modal grade for 15-year-olds&gt;: Openness to intercultural experiences</t>
+  </si>
+  <si>
+    <t>SC167Q04HA</t>
+  </si>
+  <si>
+    <t>Curriculum for the following in &lt;national modal grade for 15-year-olds&gt;: Respect for cultural diversity</t>
+  </si>
+  <si>
+    <t>SC167Q05HA</t>
+  </si>
+  <si>
+    <t>Curriculum for the following in &lt;national modal grade for 15-year-olds&gt;: Foreign languages</t>
+  </si>
+  <si>
+    <t>SC167Q06HA</t>
+  </si>
+  <si>
+    <t>Curriculum for the following in &lt;national modal grade for 15-year-olds&gt;: Critical thinking skills</t>
+  </si>
+  <si>
+    <t>SC158Q01HA</t>
+  </si>
+  <si>
+    <t>Formal curriculum in &lt;national modal grade for 15-year-olds&gt;: Climate change and global warming</t>
+  </si>
+  <si>
+    <t>SC158Q02HA</t>
+  </si>
+  <si>
+    <t>Formal curriculum in &lt;national modal grade for 15-year-olds&gt;: Global health (e.g. epidemics)</t>
+  </si>
+  <si>
+    <t>SC158Q04HA</t>
+  </si>
+  <si>
+    <t>Formal curriculum in &lt;national modal grade for 15-year-olds&gt;: Migration (movement of people)</t>
+  </si>
+  <si>
+    <t>SC158Q07HA</t>
+  </si>
+  <si>
+    <t>Formal curriculum in &lt;national modal grade for 15-year-olds&gt;: International conflicts</t>
+  </si>
+  <si>
+    <t>SC158Q08HA</t>
+  </si>
+  <si>
+    <t>Formal curriculum in &lt;national modal grade for 15-year-olds&gt;: Hunger or malnutrition in different parts of the world</t>
+  </si>
+  <si>
+    <t>SC158Q09HA</t>
+  </si>
+  <si>
+    <t>Formal curriculum in &lt;national modal grade for 15-year-olds&gt;: Causes of poverty</t>
+  </si>
+  <si>
+    <t>SC158Q12HA</t>
+  </si>
+  <si>
+    <t>Formal curriculum in &lt;national modal grade for 15-year-olds&gt;: Equality between men and women in [...] the world</t>
+  </si>
+  <si>
+    <t>SC061Q01TA</t>
+  </si>
+  <si>
+    <t>Extent to which student learning is hindered by: Student truancy</t>
+  </si>
+  <si>
+    <t>SC061Q02TA</t>
+  </si>
+  <si>
+    <t>Extent to which student learning is hindered by: Students skipping classes</t>
+  </si>
+  <si>
+    <t>SC061Q03TA</t>
+  </si>
+  <si>
+    <t>Extent to which student learning is hindered by: Students lacking respect for teachers</t>
+  </si>
+  <si>
+    <t>SC061Q04TA</t>
+  </si>
+  <si>
+    <t>Extent to which student learning is hindered by: Student use of alcohol or illegal drugs</t>
+  </si>
+  <si>
+    <t>SC061Q05TA</t>
+  </si>
+  <si>
+    <t>Extent to which student learning is hindered by: Students intimidating or bullying other students</t>
+  </si>
+  <si>
+    <t>SC061Q11HA</t>
+  </si>
+  <si>
+    <t>Extent to which student learning is hindered by: Students not being attentive</t>
+  </si>
+  <si>
+    <t>SC061Q06TA</t>
+  </si>
+  <si>
+    <t>Extent to which student learning is hindered by: Teachers not meeting individual students' needs</t>
+  </si>
+  <si>
+    <t>SC061Q07TA</t>
+  </si>
+  <si>
+    <t>Extent to which student learning is hindered by: Teacher absenteeism</t>
+  </si>
+  <si>
+    <t>SC061Q08TA</t>
+  </si>
+  <si>
+    <t>Extent to which student learning is hindered by: Staff resisting change</t>
+  </si>
+  <si>
+    <t>SC061Q09TA</t>
+  </si>
+  <si>
+    <t>Extent to which student learning is hindered by: Teachers being too strict with students</t>
+  </si>
+  <si>
+    <t>SC061Q10TA</t>
+  </si>
+  <si>
+    <t>Extent to which student learning is hindered by: Teachers not being well prepared for classes</t>
+  </si>
+  <si>
+    <t>SC002Q01TA</t>
+  </si>
+  <si>
+    <t>As of &lt;February 1, 2018&gt;, what was the total school enrolment (number of students)? Number of boys</t>
+  </si>
+  <si>
+    <t>SC002Q02TA</t>
+  </si>
+  <si>
+    <t>As of &lt;February 1, 2018&gt;, what was the total school enrolment (number of students)? Number of girls</t>
+  </si>
+  <si>
+    <t>SC048Q01NA</t>
+  </si>
+  <si>
+    <t>Percentage &lt;national modal grade for 15-year-olds&gt;: Students whose &lt;heritage language&gt; is different from &lt;test language&gt;</t>
+  </si>
+  <si>
+    <t>SC048Q02NA</t>
+  </si>
+  <si>
+    <t>Percentage &lt;national modal grade for 15-year-olds&gt;: Students with special needs</t>
+  </si>
+  <si>
+    <t>SC048Q03NA</t>
+  </si>
+  <si>
+    <t>Percentage &lt;national modal grade for 15-year-olds&gt;: Students from socioeconomically disadvantaged homes</t>
+  </si>
+  <si>
+    <t>SC004Q01TA</t>
+  </si>
+  <si>
+    <t>At your school, what is the total number of students in the &lt;national modal grade for 15-year-olds&gt;?</t>
+  </si>
+  <si>
+    <t>SC004Q02TA</t>
+  </si>
+  <si>
+    <t>Approximately, how many computers are available for these students for educational purposes?</t>
+  </si>
+  <si>
+    <t>SC004Q03TA</t>
+  </si>
+  <si>
+    <t>Approximately, how many of these computers are connected to Internet/World Wide Web?</t>
+  </si>
+  <si>
+    <t>SC004Q04NA</t>
+  </si>
+  <si>
+    <t>Approximately, how many of these computers are portable (e.g. laptop, tablet)?</t>
+  </si>
+  <si>
+    <t>SC004Q05NA</t>
+  </si>
+  <si>
+    <t>Approximately, how many interactive Whiteboards are available in the school altogether?</t>
+  </si>
+  <si>
+    <t>SC004Q06NA</t>
+  </si>
+  <si>
+    <t>Approximately, how many data projectors are available in the school altogether?</t>
+  </si>
+  <si>
+    <t>SC004Q07NA</t>
+  </si>
+  <si>
+    <t>Approximately, how many computers with Internet connection are available for teachers in your school?</t>
+  </si>
+  <si>
+    <t>SC018Q01TA01</t>
+  </si>
+  <si>
+    <t>Teachers in TOTAL: Full-time</t>
+  </si>
+  <si>
+    <t>SC018Q01TA02</t>
+  </si>
+  <si>
+    <t>Teachers in TOTAL: Part-time</t>
+  </si>
+  <si>
+    <t>SC018Q02TA01</t>
+  </si>
+  <si>
+    <t>Teachers &lt;fully certified&gt; by &lt;the appropriate authority&gt;: Full-time</t>
+  </si>
+  <si>
+    <t>SC018Q02TA02</t>
+  </si>
+  <si>
+    <t>Teachers &lt;fully certified&gt; by &lt;the appropriate authority&gt;: Part-time</t>
+  </si>
+  <si>
+    <t>SC018Q05NA01</t>
+  </si>
+  <si>
+    <t>Teachers with an &lt;ISCED Level 5A Bachelor degree&gt; qualification: Full-time</t>
+  </si>
+  <si>
+    <t>SC018Q05NA02</t>
+  </si>
+  <si>
+    <t>Teachers with an &lt;ISCED Level 5A Bachelor degree&gt; qualification: Part-time</t>
+  </si>
+  <si>
+    <t>SC018Q06NA01</t>
+  </si>
+  <si>
+    <t>Teachers with an &lt;ISCED Level 5A Master's degree&gt; qualification: Full-time</t>
+  </si>
+  <si>
+    <t>SC018Q06NA02</t>
+  </si>
+  <si>
+    <t>Teachers with an &lt;ISCED Level 5A Master's degree&gt; qualification: Part-time</t>
+  </si>
+  <si>
+    <t>SC018Q07NA01</t>
+  </si>
+  <si>
+    <t>Teachers with an &lt;ISCED Level 6&gt; qualification: Full-time</t>
+  </si>
+  <si>
+    <t>SC018Q07NA02</t>
+  </si>
+  <si>
+    <t>Teachers with an &lt;ISCED Level 6&gt; qualification: Part-time</t>
+  </si>
+  <si>
+    <t>SC025Q01NA</t>
+  </si>
+  <si>
+    <t>During the last three months, what percentage of teaching staff [...] attended a programme of professional development?</t>
+  </si>
+  <si>
+    <t>SC159Q01HA</t>
+  </si>
+  <si>
+    <t>Does your school host visiting teachers from other countries?</t>
+  </si>
+  <si>
+    <t>SC003Q01TA</t>
+  </si>
+  <si>
+    <t>What is the average size of &lt;test language&gt; classes in &lt;national modal grade for 15-year-olds&gt; in your school?</t>
+  </si>
+  <si>
+    <t>SC053Q01TA</t>
+  </si>
+  <si>
+    <t>&lt;This academic year&gt;, activities offered to &lt;national modal grade for 15-year-olds&gt;: Band, orchestra or choir</t>
+  </si>
+  <si>
+    <t>SC053Q02TA</t>
+  </si>
+  <si>
+    <t>&lt;This academic year&gt;, activities offered to &lt;national modal grade for 15-year-olds&gt;: School play or school musical</t>
+  </si>
+  <si>
+    <t>SC053Q03TA</t>
+  </si>
+  <si>
+    <t>&lt;This academic year&gt;, activities offered to &lt;national modal grade for 15-year-olds&gt;: School yearbook, newspaper [...]</t>
+  </si>
+  <si>
+    <t>SC053Q04TA</t>
+  </si>
+  <si>
+    <t>&lt;This academic year&gt;, activities offered to &lt;national modal grade for 15-year-olds&gt;: Volunteering [...]</t>
+  </si>
+  <si>
+    <t>SC053Q12IA</t>
+  </si>
+  <si>
+    <t>&lt;This academic year&gt;, activities offered to &lt;national modal grade for 15-year-olds&gt;: Book club</t>
+  </si>
+  <si>
+    <t>SC053Q13IA</t>
+  </si>
+  <si>
+    <t>&lt;This academic year&gt;, activities offered to &lt;national modal grade for 15-year-olds&gt;: Debating club or debating [...]</t>
+  </si>
+  <si>
+    <t>SC053Q09TA</t>
+  </si>
+  <si>
+    <t>&lt;This academic year&gt;, activities offered to &lt;national modal grade for 15-year-olds&gt;: Art club or art activities</t>
+  </si>
+  <si>
+    <t>SC053Q10TA</t>
+  </si>
+  <si>
+    <t>&lt;This academic year&gt;, activities offered to &lt;national modal grade for 15-year-olds&gt;: Sporting team or sporting [...]</t>
+  </si>
+  <si>
+    <t>SC053Q14IA</t>
+  </si>
+  <si>
+    <t>&lt;This academic year&gt;, activities offered to &lt;national modal grade for 15-year-olds&gt;: Lectures and/or seminars [...]</t>
+  </si>
+  <si>
+    <t>SC053Q15IA</t>
+  </si>
+  <si>
+    <t>&lt;This academic year&gt;, activities offered to &lt;national modal grade for 15-year-olds&gt;: Collaboration with local libraries</t>
+  </si>
+  <si>
+    <t>SC053Q16IA</t>
+  </si>
+  <si>
+    <t>&lt;This academic year&gt;, activities offered to &lt;national modal grade for 15-year-olds&gt;: Collaboration with local newspapers</t>
+  </si>
+  <si>
+    <t>SC053D11TA</t>
+  </si>
+  <si>
+    <t>&lt;This academic year&gt;,follow. activities/school offers&lt;national modal grade for 15-year-olds&gt;? &lt;country specific item&gt;</t>
+  </si>
+  <si>
+    <t>SC150Q01IA</t>
+  </si>
+  <si>
+    <t>School's equity-oriented policies: These students attend regular classes and receive additional periods of [...]</t>
+  </si>
+  <si>
+    <t>SC150Q02IA</t>
+  </si>
+  <si>
+    <t>School's equity-oriented policies: Before transferring to regular classes, [...] preparatory programme aimed at [...]</t>
+  </si>
+  <si>
+    <t>SC150Q03IA</t>
+  </si>
+  <si>
+    <t>School's equity-oriented policies: Before transferring to regular classes, [...] instruction in school subjects [...]</t>
+  </si>
+  <si>
+    <t>SC150Q04IA</t>
+  </si>
+  <si>
+    <t>School's equity-oriented policies: These students receive [...] amounts of instruction in their &lt;heritage language&gt;</t>
+  </si>
+  <si>
+    <t>SC150Q05IA</t>
+  </si>
+  <si>
+    <t>Schools equity-oriented policies: Class size is reduced to cater to the special needs of these students.</t>
+  </si>
+  <si>
+    <t>SC164Q01HA</t>
+  </si>
+  <si>
+    <t>In the last full academic year, what proportion of students in [...] final grade left school without a &lt;certificate&gt;?</t>
+  </si>
+  <si>
+    <t>SC064Q01TA</t>
+  </si>
+  <si>
+    <t>Proportion of parents: Discussed their child's progress with a teacher on their own initiative</t>
+  </si>
+  <si>
+    <t>SC064Q02TA</t>
+  </si>
+  <si>
+    <t>Proportion of parents: Discussed their child's progress on the initiative of one of their child's teachers</t>
+  </si>
+  <si>
+    <t>SC064Q03TA</t>
+  </si>
+  <si>
+    <t>Proportion of parents: Participated in local school government (e.g. parent council or school management committee)</t>
+  </si>
+  <si>
+    <t>SC064Q04NA</t>
+  </si>
+  <si>
+    <t>Proportion of parents: Volunteered in physical or extra-curricular activities [...]</t>
+  </si>
+  <si>
+    <t>SC152Q01HA</t>
+  </si>
+  <si>
+    <t>Does your school offer additional &lt;test language&gt; lessons [...] during the usual school hours?</t>
+  </si>
+  <si>
+    <t>SC160Q01WA</t>
+  </si>
+  <si>
+    <t>What is the purpose of these additional &lt;test language&gt; lessons?</t>
+  </si>
+  <si>
+    <t>SC052Q01NA</t>
+  </si>
+  <si>
+    <t>For 15-year old students, school provides study help: Room(s) where the students can do their homework</t>
+  </si>
+  <si>
+    <t>SC052Q02NA</t>
+  </si>
+  <si>
+    <t>For 15-year old students, school provides study help: Staff help with homework</t>
+  </si>
+  <si>
+    <t>SC052Q03HA</t>
+  </si>
+  <si>
+    <t>For 15-year old students, school provides study help: Peer-to-peer tutoring</t>
+  </si>
+  <si>
+    <t>PRIVATESCH</t>
+  </si>
+  <si>
+    <t>School type derived from sampling information; values = public, private, missing</t>
+  </si>
+  <si>
+    <t>SCHLTYPE</t>
+  </si>
+  <si>
+    <t>School Ownership</t>
+  </si>
+  <si>
+    <t>STRATIO</t>
+  </si>
+  <si>
+    <t>Student-Teacher ratio</t>
+  </si>
+  <si>
+    <t>SCHSIZE</t>
+  </si>
+  <si>
+    <t>School Size (Sum)</t>
+  </si>
+  <si>
+    <t>RATCMP1</t>
+  </si>
+  <si>
+    <t>Number of available computers per student at modal grade</t>
+  </si>
+  <si>
+    <t>RATCMP2</t>
+  </si>
+  <si>
+    <t>Proportion of available computers that are connected to the Internet</t>
+  </si>
+  <si>
+    <t>TOTAT</t>
+  </si>
+  <si>
+    <t>Total number of all teachers at school</t>
+  </si>
+  <si>
+    <t>PROATCE</t>
+  </si>
+  <si>
+    <t>Index proportion of all teachers fully certified</t>
+  </si>
+  <si>
+    <t>PROAT5AB</t>
+  </si>
+  <si>
+    <t>Index proportion of all teachers ISCED LEVEL 5A Bachelor</t>
+  </si>
+  <si>
+    <t>PROAT5AM</t>
+  </si>
+  <si>
+    <t>Index proportion of all teachers ISCED LEVEL 5A Master</t>
+  </si>
+  <si>
+    <t>PROAT6</t>
+  </si>
+  <si>
+    <t>Index proportion of all teachers ISCED LEVEL 6</t>
+  </si>
+  <si>
+    <t>CLSIZE</t>
+  </si>
+  <si>
+    <t>Class Size</t>
+  </si>
+  <si>
+    <t>CREACTIV</t>
+  </si>
+  <si>
+    <t>Creative extra-curricular activities (Sum)</t>
+  </si>
+  <si>
+    <t>EDUSHORT</t>
+  </si>
+  <si>
+    <t>Shortage of educational material (WLE)</t>
+  </si>
+  <si>
+    <t>STAFFSHORT</t>
+  </si>
+  <si>
+    <t>Shortage of educational staff (WLE)</t>
+  </si>
+  <si>
+    <t>STUBEHA</t>
+  </si>
+  <si>
+    <t>Student behaviour hindering learning (WLE)</t>
+  </si>
+  <si>
+    <t>TEACHBEHA</t>
+  </si>
+  <si>
+    <t>Teacher behaviour hindering learning (WLE)</t>
+  </si>
+  <si>
+    <t>SCMCEG</t>
+  </si>
+  <si>
+    <t>School principal's view on teachers' multicultural and egalitarian beliefs (WLE)</t>
+  </si>
+  <si>
+    <t>W_SCHGRNRABWT</t>
+  </si>
+  <si>
+    <t>GRADE NONRESPONSE ADJUSTED SCHOOL BASE WEIGHT</t>
+  </si>
+  <si>
+    <t>W_FSTUWT_SCH_SUM</t>
+  </si>
+  <si>
+    <t>Sum of W_FSTUWT</t>
+  </si>
+  <si>
+    <t>NA (for some countries)</t>
   </si>
 </sst>
 </file>
@@ -7109,7 +8217,7 @@
   <dimension ref="A1:E1119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C477" sqref="C477"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75"/>
@@ -7406,6 +8514,9 @@
       <c r="B22" t="s">
         <v>1659</v>
       </c>
+      <c r="C22" s="1" t="s">
+        <v>2223</v>
+      </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7418,6 +8529,9 @@
       <c r="B23" t="s">
         <v>1657</v>
       </c>
+      <c r="C23" s="1" t="s">
+        <v>2223</v>
+      </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7430,6 +8544,9 @@
       <c r="B24" t="s">
         <v>1655</v>
       </c>
+      <c r="C24" s="1" t="s">
+        <v>2223</v>
+      </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -13731,7 +14848,7 @@
         <v>1593</v>
       </c>
       <c r="C506" s="1" t="s">
-        <v>2223</v>
+        <v>2595</v>
       </c>
       <c r="D506" s="1" t="s">
         <v>2221</v>
@@ -13749,7 +14866,7 @@
         <v>1595</v>
       </c>
       <c r="C507" s="1" t="s">
-        <v>2223</v>
+        <v>2595</v>
       </c>
       <c r="D507" s="1" t="s">
         <v>2221</v>
@@ -21206,4 +22323,1611 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3918117-006D-4ADF-8B53-EA27F0E01106}">
+  <dimension ref="A1:E197"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75"/>
+  <cols>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="101.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.2265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>2219</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2218</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2226</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2222</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>2227</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2227</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>2228</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2229</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>2230</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>2232</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>2234</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2235</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>2236</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>2238</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>2240</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2241</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>2242</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>2244</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>2246</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2247</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>2248</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2249</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>2250</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2251</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2253</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>2254</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2255</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>2256</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>2258</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>2260</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2261</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>2262</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2263</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>2264</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2265</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>2266</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>2268</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2269</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>2270</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2271</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>2272</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2273</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>2274</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2275</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>2276</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2277</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>2278</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2279</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>2280</v>
+      </c>
+      <c r="B38" t="s">
+        <v>2281</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>2282</v>
+      </c>
+      <c r="B39" t="s">
+        <v>2283</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>2284</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2285</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>2286</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2287</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>2288</v>
+      </c>
+      <c r="B42" t="s">
+        <v>2289</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>2290</v>
+      </c>
+      <c r="B43" t="s">
+        <v>2291</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>2292</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2293</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>2294</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2295</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>2296</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2297</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>2298</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2299</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>2300</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2301</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>2302</v>
+      </c>
+      <c r="B49" t="s">
+        <v>2303</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>2304</v>
+      </c>
+      <c r="B50" t="s">
+        <v>2305</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>2306</v>
+      </c>
+      <c r="B51" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>2309</v>
+      </c>
+      <c r="B53" t="s">
+        <v>2310</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>2311</v>
+      </c>
+      <c r="B54" t="s">
+        <v>2312</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>2313</v>
+      </c>
+      <c r="B55" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>2315</v>
+      </c>
+      <c r="B56" t="s">
+        <v>2316</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>2317</v>
+      </c>
+      <c r="B57" t="s">
+        <v>2318</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>2319</v>
+      </c>
+      <c r="B58" t="s">
+        <v>2320</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>2321</v>
+      </c>
+      <c r="B59" t="s">
+        <v>2322</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>2323</v>
+      </c>
+      <c r="B60" t="s">
+        <v>2324</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>2325</v>
+      </c>
+      <c r="B61" t="s">
+        <v>2326</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>2327</v>
+      </c>
+      <c r="B62" t="s">
+        <v>2328</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>2329</v>
+      </c>
+      <c r="B63" t="s">
+        <v>2330</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>2331</v>
+      </c>
+      <c r="B64" t="s">
+        <v>2332</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>2333</v>
+      </c>
+      <c r="B65" t="s">
+        <v>2334</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>2335</v>
+      </c>
+      <c r="B66" t="s">
+        <v>2336</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>2337</v>
+      </c>
+      <c r="B67" t="s">
+        <v>2338</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>2339</v>
+      </c>
+      <c r="B68" t="s">
+        <v>2340</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>2341</v>
+      </c>
+      <c r="B69" t="s">
+        <v>2342</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>2343</v>
+      </c>
+      <c r="B70" t="s">
+        <v>2344</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>2345</v>
+      </c>
+      <c r="B71" t="s">
+        <v>2346</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>2347</v>
+      </c>
+      <c r="B72" t="s">
+        <v>2348</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>2349</v>
+      </c>
+      <c r="B73" t="s">
+        <v>2350</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>2351</v>
+      </c>
+      <c r="B74" t="s">
+        <v>2352</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>2353</v>
+      </c>
+      <c r="B75" t="s">
+        <v>2354</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>2355</v>
+      </c>
+      <c r="B76" t="s">
+        <v>2356</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>2357</v>
+      </c>
+      <c r="B77" t="s">
+        <v>2358</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>2359</v>
+      </c>
+      <c r="B78" t="s">
+        <v>2360</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>2361</v>
+      </c>
+      <c r="B79" t="s">
+        <v>2362</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>2363</v>
+      </c>
+      <c r="B80" t="s">
+        <v>2364</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>2365</v>
+      </c>
+      <c r="B81" t="s">
+        <v>2366</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>2367</v>
+      </c>
+      <c r="B82" t="s">
+        <v>2368</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>2369</v>
+      </c>
+      <c r="B83" t="s">
+        <v>2370</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>2371</v>
+      </c>
+      <c r="B84" t="s">
+        <v>2372</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>2373</v>
+      </c>
+      <c r="B85" t="s">
+        <v>2374</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>2375</v>
+      </c>
+      <c r="B86" t="s">
+        <v>2376</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>2377</v>
+      </c>
+      <c r="B87" t="s">
+        <v>2378</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>2379</v>
+      </c>
+      <c r="B88" t="s">
+        <v>2380</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>2381</v>
+      </c>
+      <c r="B89" t="s">
+        <v>2382</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>2383</v>
+      </c>
+      <c r="B90" t="s">
+        <v>2384</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>2385</v>
+      </c>
+      <c r="B91" t="s">
+        <v>2386</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>2387</v>
+      </c>
+      <c r="B92" t="s">
+        <v>2388</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>2389</v>
+      </c>
+      <c r="B93" t="s">
+        <v>2390</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>2391</v>
+      </c>
+      <c r="B94" t="s">
+        <v>2392</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>2393</v>
+      </c>
+      <c r="B95" t="s">
+        <v>2394</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>2395</v>
+      </c>
+      <c r="B96" t="s">
+        <v>2396</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>2397</v>
+      </c>
+      <c r="B97" t="s">
+        <v>2398</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>2399</v>
+      </c>
+      <c r="B98" t="s">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>2401</v>
+      </c>
+      <c r="B99" t="s">
+        <v>2402</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>2403</v>
+      </c>
+      <c r="B100" t="s">
+        <v>2404</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>2405</v>
+      </c>
+      <c r="B101" t="s">
+        <v>2406</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>2407</v>
+      </c>
+      <c r="B102" t="s">
+        <v>2408</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>2409</v>
+      </c>
+      <c r="B103" t="s">
+        <v>2410</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>2411</v>
+      </c>
+      <c r="B104" t="s">
+        <v>2412</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>2413</v>
+      </c>
+      <c r="B105" t="s">
+        <v>2414</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>2415</v>
+      </c>
+      <c r="B106" t="s">
+        <v>2416</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>2417</v>
+      </c>
+      <c r="B107" t="s">
+        <v>2418</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>2419</v>
+      </c>
+      <c r="B108" t="s">
+        <v>2420</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>2421</v>
+      </c>
+      <c r="B109" t="s">
+        <v>2422</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>2423</v>
+      </c>
+      <c r="B110" t="s">
+        <v>2424</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>2425</v>
+      </c>
+      <c r="B111" t="s">
+        <v>2426</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>2427</v>
+      </c>
+      <c r="B112" t="s">
+        <v>2428</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>2429</v>
+      </c>
+      <c r="B113" t="s">
+        <v>2430</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>2431</v>
+      </c>
+      <c r="B114" t="s">
+        <v>2432</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>2433</v>
+      </c>
+      <c r="B115" t="s">
+        <v>2434</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>2435</v>
+      </c>
+      <c r="B116" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>2437</v>
+      </c>
+      <c r="B117" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>2439</v>
+      </c>
+      <c r="B118" t="s">
+        <v>2440</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>2441</v>
+      </c>
+      <c r="B119" t="s">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>2443</v>
+      </c>
+      <c r="B120" t="s">
+        <v>2444</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>2445</v>
+      </c>
+      <c r="B121" t="s">
+        <v>2446</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>2447</v>
+      </c>
+      <c r="B122" t="s">
+        <v>2448</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>2449</v>
+      </c>
+      <c r="B123" t="s">
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>2451</v>
+      </c>
+      <c r="B124" t="s">
+        <v>2452</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>2453</v>
+      </c>
+      <c r="B125" t="s">
+        <v>2454</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" t="s">
+        <v>2455</v>
+      </c>
+      <c r="B126" t="s">
+        <v>2456</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" t="s">
+        <v>2457</v>
+      </c>
+      <c r="B127" t="s">
+        <v>2458</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" t="s">
+        <v>2459</v>
+      </c>
+      <c r="B128" t="s">
+        <v>2460</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" t="s">
+        <v>2461</v>
+      </c>
+      <c r="B129" t="s">
+        <v>2462</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" t="s">
+        <v>2463</v>
+      </c>
+      <c r="B130" t="s">
+        <v>2464</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" t="s">
+        <v>2465</v>
+      </c>
+      <c r="B131" t="s">
+        <v>2466</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" t="s">
+        <v>2467</v>
+      </c>
+      <c r="B132" t="s">
+        <v>2468</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" t="s">
+        <v>2469</v>
+      </c>
+      <c r="B133" t="s">
+        <v>2470</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" t="s">
+        <v>2471</v>
+      </c>
+      <c r="B134" t="s">
+        <v>2472</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" t="s">
+        <v>2473</v>
+      </c>
+      <c r="B135" t="s">
+        <v>2474</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" t="s">
+        <v>2475</v>
+      </c>
+      <c r="B136" t="s">
+        <v>2476</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" t="s">
+        <v>2477</v>
+      </c>
+      <c r="B137" t="s">
+        <v>2478</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" t="s">
+        <v>2479</v>
+      </c>
+      <c r="B138" t="s">
+        <v>2480</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" t="s">
+        <v>2481</v>
+      </c>
+      <c r="B139" t="s">
+        <v>2482</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" t="s">
+        <v>2483</v>
+      </c>
+      <c r="B140" t="s">
+        <v>2484</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" t="s">
+        <v>2485</v>
+      </c>
+      <c r="B141" t="s">
+        <v>2486</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" t="s">
+        <v>2487</v>
+      </c>
+      <c r="B142" t="s">
+        <v>2488</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" t="s">
+        <v>2489</v>
+      </c>
+      <c r="B143" t="s">
+        <v>2490</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" t="s">
+        <v>2491</v>
+      </c>
+      <c r="B144" t="s">
+        <v>2492</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" t="s">
+        <v>2493</v>
+      </c>
+      <c r="B145" t="s">
+        <v>2494</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" t="s">
+        <v>2495</v>
+      </c>
+      <c r="B146" t="s">
+        <v>2496</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" t="s">
+        <v>2497</v>
+      </c>
+      <c r="B147" t="s">
+        <v>2498</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" t="s">
+        <v>2499</v>
+      </c>
+      <c r="B148" t="s">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" t="s">
+        <v>2501</v>
+      </c>
+      <c r="B149" t="s">
+        <v>2502</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" t="s">
+        <v>2503</v>
+      </c>
+      <c r="B150" t="s">
+        <v>2504</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" t="s">
+        <v>2505</v>
+      </c>
+      <c r="B151" t="s">
+        <v>2506</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" t="s">
+        <v>2507</v>
+      </c>
+      <c r="B152" t="s">
+        <v>2508</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" t="s">
+        <v>2509</v>
+      </c>
+      <c r="B153" t="s">
+        <v>2510</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" t="s">
+        <v>2511</v>
+      </c>
+      <c r="B154" t="s">
+        <v>2512</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" t="s">
+        <v>2513</v>
+      </c>
+      <c r="B155" t="s">
+        <v>2514</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" t="s">
+        <v>2515</v>
+      </c>
+      <c r="B156" t="s">
+        <v>2516</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" t="s">
+        <v>2517</v>
+      </c>
+      <c r="B157" t="s">
+        <v>2518</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" t="s">
+        <v>2519</v>
+      </c>
+      <c r="B158" t="s">
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" t="s">
+        <v>2521</v>
+      </c>
+      <c r="B159" t="s">
+        <v>2522</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" t="s">
+        <v>2523</v>
+      </c>
+      <c r="B160" t="s">
+        <v>2524</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" t="s">
+        <v>2525</v>
+      </c>
+      <c r="B161" t="s">
+        <v>2526</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162" t="s">
+        <v>2527</v>
+      </c>
+      <c r="B162" t="s">
+        <v>2528</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" t="s">
+        <v>2529</v>
+      </c>
+      <c r="B163" t="s">
+        <v>2530</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" t="s">
+        <v>2531</v>
+      </c>
+      <c r="B164" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165" t="s">
+        <v>2533</v>
+      </c>
+      <c r="B165" t="s">
+        <v>2534</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="A166" t="s">
+        <v>2535</v>
+      </c>
+      <c r="B166" t="s">
+        <v>2536</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167" t="s">
+        <v>2537</v>
+      </c>
+      <c r="B167" t="s">
+        <v>2538</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168" t="s">
+        <v>2539</v>
+      </c>
+      <c r="B168" t="s">
+        <v>2540</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="A169" t="s">
+        <v>2541</v>
+      </c>
+      <c r="B169" t="s">
+        <v>2542</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170" t="s">
+        <v>2543</v>
+      </c>
+      <c r="B170" t="s">
+        <v>2544</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171" t="s">
+        <v>2545</v>
+      </c>
+      <c r="B171" t="s">
+        <v>2546</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="A172" t="s">
+        <v>2547</v>
+      </c>
+      <c r="B172" t="s">
+        <v>2548</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="A173" t="s">
+        <v>2549</v>
+      </c>
+      <c r="B173" t="s">
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174" t="s">
+        <v>2551</v>
+      </c>
+      <c r="B174" t="s">
+        <v>2552</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
+      <c r="A175" t="s">
+        <v>2553</v>
+      </c>
+      <c r="B175" t="s">
+        <v>2554</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="A176" t="s">
+        <v>2555</v>
+      </c>
+      <c r="B176" t="s">
+        <v>2556</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177" t="s">
+        <v>2557</v>
+      </c>
+      <c r="B177" t="s">
+        <v>2558</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" t="s">
+        <v>2559</v>
+      </c>
+      <c r="B178" t="s">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" t="s">
+        <v>2561</v>
+      </c>
+      <c r="B179" t="s">
+        <v>2562</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180" t="s">
+        <v>2563</v>
+      </c>
+      <c r="B180" t="s">
+        <v>2564</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="A181" t="s">
+        <v>2565</v>
+      </c>
+      <c r="B181" t="s">
+        <v>2566</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182" t="s">
+        <v>2567</v>
+      </c>
+      <c r="B182" t="s">
+        <v>2568</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="A183" t="s">
+        <v>2569</v>
+      </c>
+      <c r="B183" t="s">
+        <v>2570</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="A184" t="s">
+        <v>2571</v>
+      </c>
+      <c r="B184" t="s">
+        <v>2572</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
+      <c r="A185" t="s">
+        <v>2573</v>
+      </c>
+      <c r="B185" t="s">
+        <v>2574</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
+      <c r="A186" t="s">
+        <v>2575</v>
+      </c>
+      <c r="B186" t="s">
+        <v>2576</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2">
+      <c r="A187" t="s">
+        <v>2577</v>
+      </c>
+      <c r="B187" t="s">
+        <v>2578</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2">
+      <c r="A188" t="s">
+        <v>2579</v>
+      </c>
+      <c r="B188" t="s">
+        <v>2580</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2">
+      <c r="A189" t="s">
+        <v>2581</v>
+      </c>
+      <c r="B189" t="s">
+        <v>2582</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
+      <c r="A190" t="s">
+        <v>2583</v>
+      </c>
+      <c r="B190" t="s">
+        <v>2584</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2">
+      <c r="A191" t="s">
+        <v>2585</v>
+      </c>
+      <c r="B191" t="s">
+        <v>2586</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
+      <c r="A192" t="s">
+        <v>2587</v>
+      </c>
+      <c r="B192" t="s">
+        <v>2588</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
+      <c r="A193" t="s">
+        <v>2589</v>
+      </c>
+      <c r="B193" t="s">
+        <v>2590</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194" t="s">
+        <v>2591</v>
+      </c>
+      <c r="B194" t="s">
+        <v>2592</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
+      <c r="A195" t="s">
+        <v>2593</v>
+      </c>
+      <c r="B195" t="s">
+        <v>2594</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
+      <c r="A196" t="s">
+        <v>2214</v>
+      </c>
+      <c r="B196" t="s">
+        <v>2215</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
+      <c r="A197" t="s">
+        <v>2216</v>
+      </c>
+      <c r="B197" t="s">
+        <v>2217</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Segnato alcune variabili come "potential" nel file excel  - Aggiunto script: 'manova_of_countries' in MANOVA (semplice confronto per vedere performance di ciascuno stato)
</commit_message>
<xml_diff>
--- a/Info and data/Features and meanings.xlsx
+++ b/Info and data/Features and meanings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\GitHub\Applied-Statistics-Project\Info and data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APPLIED\GITHUB\Applied-Statistics-Project\Info and data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC65048D-34E5-4973-ACA6-925454F08E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86259183-3F50-46FE-85A1-0A1285245350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{3DA52822-CFDA-408E-B1C3-39FC0A4F79A9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3DA52822-CFDA-408E-B1C3-39FC0A4F79A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Student features and meanings" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2857" uniqueCount="2596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2870" uniqueCount="2596">
   <si>
     <t>CNTRYID</t>
   </si>
@@ -8216,16 +8216,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F913139-5BD2-4A68-816A-F8D58E27C68E}">
   <dimension ref="A1:E1119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A625" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C950" sqref="C950"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="104.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.1328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.31640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8841,6 +8841,9 @@
       <c r="B46" t="s">
         <v>865</v>
       </c>
+      <c r="C46" s="1" t="s">
+        <v>2223</v>
+      </c>
       <c r="E46" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -12894,6 +12897,9 @@
       <c r="B378" t="s">
         <v>1365</v>
       </c>
+      <c r="C378" s="1" t="s">
+        <v>2223</v>
+      </c>
       <c r="D378" s="1" t="s">
         <v>2221</v>
       </c>
@@ -12939,6 +12945,9 @@
       <c r="B381" t="s">
         <v>1371</v>
       </c>
+      <c r="C381" s="1" t="s">
+        <v>2223</v>
+      </c>
       <c r="D381" s="1" t="s">
         <v>2221</v>
       </c>
@@ -12969,6 +12978,9 @@
       <c r="B383" t="s">
         <v>1375</v>
       </c>
+      <c r="C383" s="1" t="s">
+        <v>2223</v>
+      </c>
       <c r="D383" s="1" t="s">
         <v>2221</v>
       </c>
@@ -12984,6 +12996,9 @@
       <c r="B384" t="s">
         <v>1377</v>
       </c>
+      <c r="C384" s="1" t="s">
+        <v>2223</v>
+      </c>
       <c r="D384" s="1" t="s">
         <v>2221</v>
       </c>
@@ -12999,6 +13014,9 @@
       <c r="B385" t="s">
         <v>1409</v>
       </c>
+      <c r="C385" s="1" t="s">
+        <v>2223</v>
+      </c>
       <c r="D385" s="1" t="s">
         <v>2221</v>
       </c>
@@ -13014,6 +13032,9 @@
       <c r="B386" t="s">
         <v>1411</v>
       </c>
+      <c r="C386" s="1" t="s">
+        <v>2223</v>
+      </c>
       <c r="D386" s="1" t="s">
         <v>2221</v>
       </c>
@@ -13164,6 +13185,9 @@
       <c r="B396" t="s">
         <v>1499</v>
       </c>
+      <c r="C396" s="1" t="s">
+        <v>2223</v>
+      </c>
       <c r="D396" s="1" t="s">
         <v>2221</v>
       </c>
@@ -13434,6 +13458,9 @@
       <c r="B414" t="s">
         <v>1479</v>
       </c>
+      <c r="C414" s="1" t="s">
+        <v>2223</v>
+      </c>
       <c r="D414" s="1" t="s">
         <v>2221</v>
       </c>
@@ -13872,6 +13899,9 @@
       <c r="B441" t="s">
         <v>1637</v>
       </c>
+      <c r="C441" s="1" t="s">
+        <v>2223</v>
+      </c>
       <c r="D441" s="1" t="s">
         <v>2221</v>
       </c>
@@ -15282,6 +15312,9 @@
       <c r="B536" t="s">
         <v>2053</v>
       </c>
+      <c r="C536" s="1" t="s">
+        <v>2223</v>
+      </c>
       <c r="E536" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -15390,6 +15423,9 @@
       <c r="B545" t="s">
         <v>2035</v>
       </c>
+      <c r="C545" s="1" t="s">
+        <v>2223</v>
+      </c>
       <c r="E545" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -18764,6 +18800,9 @@
       </c>
       <c r="B824" t="s">
         <v>387</v>
+      </c>
+      <c r="C824" s="1" t="s">
+        <v>2223</v>
       </c>
       <c r="E824" t="str">
         <f t="shared" si="12"/>
@@ -22333,13 +22372,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
-    <col min="2" max="2" width="101.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.2265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="101.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>

<commit_message>
Updated features / started manova of school from lmer
</commit_message>
<xml_diff>
--- a/Info and data/Features and meanings.xlsx
+++ b/Info and data/Features and meanings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APPLIED\GITHUB\Applied-Statistics-Project\Info and data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\GitHub\Applied-Statistics-Project\Info and data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13275CF6-A05A-4494-B69C-E695DE0DDAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0B0336-F3B0-4A93-9CDE-CCC0D4A2F4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3DA52822-CFDA-408E-B1C3-39FC0A4F79A9}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="1" xr2:uid="{3DA52822-CFDA-408E-B1C3-39FC0A4F79A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Student features and meanings" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4018" uniqueCount="2603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4019" uniqueCount="2603">
   <si>
     <t>CNTRYID</t>
   </si>
@@ -8248,20 +8248,20 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H1119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A563" sqref="A563"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="104.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.2265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.08984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.31640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
     <col min="6" max="6" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.21875" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2265625" customWidth="1"/>
+    <col min="8" max="8" width="22.31640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -25794,19 +25794,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3918117-006D-4ADF-8B53-EA27F0E01106}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:D197"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C187" sqref="C187"/>
+    <sheetView tabSelected="1" topLeftCell="A164" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C177" sqref="C177"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
-    <col min="2" max="2" width="101.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" customWidth="1"/>
+    <col min="2" max="2" width="101.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.76953125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -25823,7 +25822,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -25835,7 +25834,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -25847,7 +25846,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -25859,7 +25858,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -25871,7 +25870,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -25883,7 +25882,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>2227</v>
       </c>
@@ -25895,7 +25894,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -25907,7 +25906,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -25919,7 +25918,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -25931,7 +25930,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -25943,7 +25942,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>2228</v>
       </c>
@@ -25955,7 +25954,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>2230</v>
       </c>
@@ -25967,7 +25966,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>2232</v>
       </c>
@@ -25979,7 +25978,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>2234</v>
       </c>
@@ -25991,7 +25990,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>2236</v>
       </c>
@@ -26003,7 +26002,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>2238</v>
       </c>
@@ -26015,7 +26014,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>2240</v>
       </c>
@@ -26027,7 +26026,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>2242</v>
       </c>
@@ -26039,7 +26038,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>2244</v>
       </c>
@@ -26051,7 +26050,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>2246</v>
       </c>
@@ -26063,7 +26062,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>2248</v>
       </c>
@@ -26075,7 +26074,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>2250</v>
       </c>
@@ -26087,7 +26086,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>2252</v>
       </c>
@@ -26099,7 +26098,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>2254</v>
       </c>
@@ -26111,7 +26110,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>2256</v>
       </c>
@@ -26123,7 +26122,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>2258</v>
       </c>
@@ -26135,7 +26134,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>2260</v>
       </c>
@@ -26147,7 +26146,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>2262</v>
       </c>
@@ -26159,7 +26158,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>2264</v>
       </c>
@@ -26171,7 +26170,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:4" hidden="1">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>2266</v>
       </c>
@@ -26183,7 +26182,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>2268</v>
       </c>
@@ -26195,7 +26194,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>2270</v>
       </c>
@@ -26207,7 +26206,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>2272</v>
       </c>
@@ -26219,7 +26218,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>2274</v>
       </c>
@@ -26231,7 +26230,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:4" hidden="1">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>2276</v>
       </c>
@@ -26243,7 +26242,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:4" hidden="1">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>2278</v>
       </c>
@@ -26255,7 +26254,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:4" hidden="1">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>2280</v>
       </c>
@@ -26267,7 +26266,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:4" hidden="1">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>2282</v>
       </c>
@@ -26279,7 +26278,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:4" hidden="1">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>2284</v>
       </c>
@@ -26291,7 +26290,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:4" hidden="1">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>2286</v>
       </c>
@@ -26303,7 +26302,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:4" hidden="1">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>2288</v>
       </c>
@@ -26315,7 +26314,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:4" hidden="1">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>2290</v>
       </c>
@@ -26327,7 +26326,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:4" hidden="1">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>2292</v>
       </c>
@@ -26339,7 +26338,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:4" hidden="1">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>2294</v>
       </c>
@@ -26351,7 +26350,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:4" hidden="1">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>2296</v>
       </c>
@@ -26363,7 +26362,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1">
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>2298</v>
       </c>
@@ -26375,7 +26374,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>2300</v>
       </c>
@@ -26387,7 +26386,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>2302</v>
       </c>
@@ -26399,7 +26398,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:4" hidden="1">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>2304</v>
       </c>
@@ -26411,7 +26410,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>2306</v>
       </c>
@@ -26423,7 +26422,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:4" hidden="1">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>2308</v>
       </c>
@@ -26435,7 +26434,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:4" hidden="1">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>2309</v>
       </c>
@@ -26447,7 +26446,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:4" hidden="1">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>2311</v>
       </c>
@@ -26459,7 +26458,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:4" hidden="1">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>2313</v>
       </c>
@@ -26471,7 +26470,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:4" hidden="1">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>2315</v>
       </c>
@@ -26483,7 +26482,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:4" hidden="1">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>2317</v>
       </c>
@@ -26495,7 +26494,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:4" hidden="1">
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>2319</v>
       </c>
@@ -26507,7 +26506,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:4" hidden="1">
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>2321</v>
       </c>
@@ -26519,7 +26518,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:4" hidden="1">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>2323</v>
       </c>
@@ -26531,7 +26530,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:4" hidden="1">
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
         <v>2325</v>
       </c>
@@ -26543,7 +26542,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:4" hidden="1">
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>2327</v>
       </c>
@@ -26555,7 +26554,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:4" hidden="1">
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>2329</v>
       </c>
@@ -26567,7 +26566,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:4" hidden="1">
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
         <v>2331</v>
       </c>
@@ -26579,7 +26578,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:4" hidden="1">
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>2333</v>
       </c>
@@ -26591,7 +26590,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:4" hidden="1">
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>2335</v>
       </c>
@@ -26603,7 +26602,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:4" hidden="1">
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>2337</v>
       </c>
@@ -26615,7 +26614,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:4" hidden="1">
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>2339</v>
       </c>
@@ -26627,7 +26626,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:4" hidden="1">
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>2341</v>
       </c>
@@ -26639,7 +26638,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:4" hidden="1">
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>2343</v>
       </c>
@@ -26651,7 +26650,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:4" hidden="1">
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>2345</v>
       </c>
@@ -26663,7 +26662,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:4" hidden="1">
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>2347</v>
       </c>
@@ -26675,7 +26674,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:4" hidden="1">
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>2349</v>
       </c>
@@ -26687,7 +26686,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:4" hidden="1">
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>2351</v>
       </c>
@@ -26699,7 +26698,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:4" hidden="1">
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>2353</v>
       </c>
@@ -26711,7 +26710,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:4" hidden="1">
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>2355</v>
       </c>
@@ -26723,7 +26722,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:4" hidden="1">
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
         <v>2357</v>
       </c>
@@ -26735,7 +26734,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:4" hidden="1">
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>2359</v>
       </c>
@@ -26747,7 +26746,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:4" hidden="1">
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
         <v>2361</v>
       </c>
@@ -26759,7 +26758,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:4" hidden="1">
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>2363</v>
       </c>
@@ -26771,7 +26770,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:4" hidden="1">
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
         <v>2365</v>
       </c>
@@ -26783,7 +26782,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:4" hidden="1">
+    <row r="82" spans="1:4">
       <c r="A82" t="s">
         <v>2367</v>
       </c>
@@ -26795,7 +26794,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:4" hidden="1">
+    <row r="83" spans="1:4">
       <c r="A83" t="s">
         <v>2369</v>
       </c>
@@ -26807,7 +26806,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:4" hidden="1">
+    <row r="84" spans="1:4">
       <c r="A84" t="s">
         <v>2371</v>
       </c>
@@ -26819,7 +26818,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:4" hidden="1">
+    <row r="85" spans="1:4">
       <c r="A85" t="s">
         <v>2373</v>
       </c>
@@ -26906,7 +26905,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:4" hidden="1">
+    <row r="91" spans="1:4">
       <c r="A91" t="s">
         <v>2385</v>
       </c>
@@ -27038,7 +27037,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:4" hidden="1">
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
         <v>2403</v>
       </c>
@@ -27050,7 +27049,7 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="1:4" hidden="1">
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
         <v>2405</v>
       </c>
@@ -27062,7 +27061,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="1:4" hidden="1">
+    <row r="102" spans="1:4">
       <c r="A102" t="s">
         <v>2407</v>
       </c>
@@ -27074,7 +27073,7 @@
         <v/>
       </c>
     </row>
-    <row r="103" spans="1:4" hidden="1">
+    <row r="103" spans="1:4">
       <c r="A103" t="s">
         <v>2409</v>
       </c>
@@ -27086,7 +27085,7 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:4" hidden="1">
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
         <v>2411</v>
       </c>
@@ -27098,7 +27097,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:4" hidden="1">
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
         <v>2413</v>
       </c>
@@ -27110,7 +27109,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:4" hidden="1">
+    <row r="106" spans="1:4">
       <c r="A106" t="s">
         <v>2415</v>
       </c>
@@ -27122,7 +27121,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:4" hidden="1">
+    <row r="107" spans="1:4">
       <c r="A107" t="s">
         <v>2417</v>
       </c>
@@ -27134,7 +27133,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:4" hidden="1">
+    <row r="108" spans="1:4">
       <c r="A108" t="s">
         <v>2419</v>
       </c>
@@ -27146,7 +27145,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:4" hidden="1">
+    <row r="109" spans="1:4">
       <c r="A109" t="s">
         <v>2421</v>
       </c>
@@ -27158,7 +27157,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:4" hidden="1">
+    <row r="110" spans="1:4">
       <c r="A110" t="s">
         <v>2423</v>
       </c>
@@ -27170,7 +27169,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="1:4" hidden="1">
+    <row r="111" spans="1:4">
       <c r="A111" t="s">
         <v>2425</v>
       </c>
@@ -27182,7 +27181,7 @@
         <v/>
       </c>
     </row>
-    <row r="112" spans="1:4" hidden="1">
+    <row r="112" spans="1:4">
       <c r="A112" t="s">
         <v>2427</v>
       </c>
@@ -27194,7 +27193,7 @@
         <v/>
       </c>
     </row>
-    <row r="113" spans="1:4" hidden="1">
+    <row r="113" spans="1:4">
       <c r="A113" t="s">
         <v>2429</v>
       </c>
@@ -27206,7 +27205,7 @@
         <v/>
       </c>
     </row>
-    <row r="114" spans="1:4" hidden="1">
+    <row r="114" spans="1:4">
       <c r="A114" t="s">
         <v>2431</v>
       </c>
@@ -27218,7 +27217,7 @@
         <v/>
       </c>
     </row>
-    <row r="115" spans="1:4" hidden="1">
+    <row r="115" spans="1:4">
       <c r="A115" t="s">
         <v>2433</v>
       </c>
@@ -27230,7 +27229,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:4" hidden="1">
+    <row r="116" spans="1:4">
       <c r="A116" t="s">
         <v>2435</v>
       </c>
@@ -27242,7 +27241,7 @@
         <v/>
       </c>
     </row>
-    <row r="117" spans="1:4" hidden="1">
+    <row r="117" spans="1:4">
       <c r="A117" t="s">
         <v>2437</v>
       </c>
@@ -27254,7 +27253,7 @@
         <v/>
       </c>
     </row>
-    <row r="118" spans="1:4" hidden="1">
+    <row r="118" spans="1:4">
       <c r="A118" t="s">
         <v>2439</v>
       </c>
@@ -27266,7 +27265,7 @@
         <v/>
       </c>
     </row>
-    <row r="119" spans="1:4" hidden="1">
+    <row r="119" spans="1:4">
       <c r="A119" t="s">
         <v>2441</v>
       </c>
@@ -27278,7 +27277,7 @@
         <v/>
       </c>
     </row>
-    <row r="120" spans="1:4" hidden="1">
+    <row r="120" spans="1:4">
       <c r="A120" t="s">
         <v>2443</v>
       </c>
@@ -27290,7 +27289,7 @@
         <v/>
       </c>
     </row>
-    <row r="121" spans="1:4" hidden="1">
+    <row r="121" spans="1:4">
       <c r="A121" t="s">
         <v>2445</v>
       </c>
@@ -27302,7 +27301,7 @@
         <v/>
       </c>
     </row>
-    <row r="122" spans="1:4" hidden="1">
+    <row r="122" spans="1:4">
       <c r="A122" t="s">
         <v>2447</v>
       </c>
@@ -27314,7 +27313,7 @@
         <v/>
       </c>
     </row>
-    <row r="123" spans="1:4" hidden="1">
+    <row r="123" spans="1:4">
       <c r="A123" t="s">
         <v>2449</v>
       </c>
@@ -27326,7 +27325,7 @@
         <v/>
       </c>
     </row>
-    <row r="124" spans="1:4" hidden="1">
+    <row r="124" spans="1:4">
       <c r="A124" t="s">
         <v>2451</v>
       </c>
@@ -27338,7 +27337,7 @@
         <v/>
       </c>
     </row>
-    <row r="125" spans="1:4" hidden="1">
+    <row r="125" spans="1:4">
       <c r="A125" t="s">
         <v>2453</v>
       </c>
@@ -27350,7 +27349,7 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:4" hidden="1">
+    <row r="126" spans="1:4">
       <c r="A126" t="s">
         <v>2455</v>
       </c>
@@ -27362,7 +27361,7 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:4" hidden="1">
+    <row r="127" spans="1:4">
       <c r="A127" t="s">
         <v>2457</v>
       </c>
@@ -27374,7 +27373,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:4" hidden="1">
+    <row r="128" spans="1:4">
       <c r="A128" t="s">
         <v>2459</v>
       </c>
@@ -27386,7 +27385,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:4" hidden="1">
+    <row r="129" spans="1:4">
       <c r="A129" t="s">
         <v>2461</v>
       </c>
@@ -27398,7 +27397,7 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="1:4" hidden="1">
+    <row r="130" spans="1:4">
       <c r="A130" t="s">
         <v>2463</v>
       </c>
@@ -27410,7 +27409,7 @@
         <v/>
       </c>
     </row>
-    <row r="131" spans="1:4" hidden="1">
+    <row r="131" spans="1:4">
       <c r="A131" t="s">
         <v>2465</v>
       </c>
@@ -27422,7 +27421,7 @@
         <v/>
       </c>
     </row>
-    <row r="132" spans="1:4" hidden="1">
+    <row r="132" spans="1:4">
       <c r="A132" t="s">
         <v>2467</v>
       </c>
@@ -27434,7 +27433,7 @@
         <v/>
       </c>
     </row>
-    <row r="133" spans="1:4" hidden="1">
+    <row r="133" spans="1:4">
       <c r="A133" t="s">
         <v>2469</v>
       </c>
@@ -27446,7 +27445,7 @@
         <v/>
       </c>
     </row>
-    <row r="134" spans="1:4" hidden="1">
+    <row r="134" spans="1:4">
       <c r="A134" t="s">
         <v>2471</v>
       </c>
@@ -27458,7 +27457,7 @@
         <v/>
       </c>
     </row>
-    <row r="135" spans="1:4" hidden="1">
+    <row r="135" spans="1:4">
       <c r="A135" t="s">
         <v>2473</v>
       </c>
@@ -27500,7 +27499,7 @@
         <v/>
       </c>
     </row>
-    <row r="138" spans="1:4" hidden="1">
+    <row r="138" spans="1:4">
       <c r="A138" t="s">
         <v>2479</v>
       </c>
@@ -27512,7 +27511,7 @@
         <v/>
       </c>
     </row>
-    <row r="139" spans="1:4" hidden="1">
+    <row r="139" spans="1:4">
       <c r="A139" t="s">
         <v>2481</v>
       </c>
@@ -27524,7 +27523,7 @@
         <v/>
       </c>
     </row>
-    <row r="140" spans="1:4" hidden="1">
+    <row r="140" spans="1:4">
       <c r="A140" t="s">
         <v>2483</v>
       </c>
@@ -27536,7 +27535,7 @@
         <v/>
       </c>
     </row>
-    <row r="141" spans="1:4" hidden="1">
+    <row r="141" spans="1:4">
       <c r="A141" t="s">
         <v>2485</v>
       </c>
@@ -27548,7 +27547,7 @@
         <v/>
       </c>
     </row>
-    <row r="142" spans="1:4" hidden="1">
+    <row r="142" spans="1:4">
       <c r="A142" t="s">
         <v>2487</v>
       </c>
@@ -27560,7 +27559,7 @@
         <v/>
       </c>
     </row>
-    <row r="143" spans="1:4" hidden="1">
+    <row r="143" spans="1:4">
       <c r="A143" t="s">
         <v>2489</v>
       </c>
@@ -27572,7 +27571,7 @@
         <v/>
       </c>
     </row>
-    <row r="144" spans="1:4" hidden="1">
+    <row r="144" spans="1:4">
       <c r="A144" t="s">
         <v>2491</v>
       </c>
@@ -27584,7 +27583,7 @@
         <v/>
       </c>
     </row>
-    <row r="145" spans="1:4" hidden="1">
+    <row r="145" spans="1:4">
       <c r="A145" t="s">
         <v>2493</v>
       </c>
@@ -27596,7 +27595,7 @@
         <v/>
       </c>
     </row>
-    <row r="146" spans="1:4" hidden="1">
+    <row r="146" spans="1:4">
       <c r="A146" t="s">
         <v>2495</v>
       </c>
@@ -27608,7 +27607,7 @@
         <v/>
       </c>
     </row>
-    <row r="147" spans="1:4" hidden="1">
+    <row r="147" spans="1:4">
       <c r="A147" t="s">
         <v>2497</v>
       </c>
@@ -27620,7 +27619,7 @@
         <v/>
       </c>
     </row>
-    <row r="148" spans="1:4" hidden="1">
+    <row r="148" spans="1:4">
       <c r="A148" t="s">
         <v>2499</v>
       </c>
@@ -27632,7 +27631,7 @@
         <v/>
       </c>
     </row>
-    <row r="149" spans="1:4" hidden="1">
+    <row r="149" spans="1:4">
       <c r="A149" t="s">
         <v>2501</v>
       </c>
@@ -27644,7 +27643,7 @@
         <v/>
       </c>
     </row>
-    <row r="150" spans="1:4" hidden="1">
+    <row r="150" spans="1:4">
       <c r="A150" t="s">
         <v>2503</v>
       </c>
@@ -27656,7 +27655,7 @@
         <v/>
       </c>
     </row>
-    <row r="151" spans="1:4" hidden="1">
+    <row r="151" spans="1:4">
       <c r="A151" t="s">
         <v>2505</v>
       </c>
@@ -27668,7 +27667,7 @@
         <v/>
       </c>
     </row>
-    <row r="152" spans="1:4" hidden="1">
+    <row r="152" spans="1:4">
       <c r="A152" t="s">
         <v>2507</v>
       </c>
@@ -27680,7 +27679,7 @@
         <v/>
       </c>
     </row>
-    <row r="153" spans="1:4" hidden="1">
+    <row r="153" spans="1:4">
       <c r="A153" t="s">
         <v>2509</v>
       </c>
@@ -27692,7 +27691,7 @@
         <v/>
       </c>
     </row>
-    <row r="154" spans="1:4" hidden="1">
+    <row r="154" spans="1:4">
       <c r="A154" t="s">
         <v>2511</v>
       </c>
@@ -27704,7 +27703,7 @@
         <v/>
       </c>
     </row>
-    <row r="155" spans="1:4" hidden="1">
+    <row r="155" spans="1:4">
       <c r="A155" t="s">
         <v>2513</v>
       </c>
@@ -27716,7 +27715,7 @@
         <v/>
       </c>
     </row>
-    <row r="156" spans="1:4" hidden="1">
+    <row r="156" spans="1:4">
       <c r="A156" t="s">
         <v>2515</v>
       </c>
@@ -27728,7 +27727,7 @@
         <v/>
       </c>
     </row>
-    <row r="157" spans="1:4" hidden="1">
+    <row r="157" spans="1:4">
       <c r="A157" t="s">
         <v>2517</v>
       </c>
@@ -27740,7 +27739,7 @@
         <v/>
       </c>
     </row>
-    <row r="158" spans="1:4" hidden="1">
+    <row r="158" spans="1:4">
       <c r="A158" t="s">
         <v>2519</v>
       </c>
@@ -27752,7 +27751,7 @@
         <v/>
       </c>
     </row>
-    <row r="159" spans="1:4" hidden="1">
+    <row r="159" spans="1:4">
       <c r="A159" t="s">
         <v>2521</v>
       </c>
@@ -27764,7 +27763,7 @@
         <v/>
       </c>
     </row>
-    <row r="160" spans="1:4" hidden="1">
+    <row r="160" spans="1:4">
       <c r="A160" t="s">
         <v>2523</v>
       </c>
@@ -27776,7 +27775,7 @@
         <v/>
       </c>
     </row>
-    <row r="161" spans="1:4" hidden="1">
+    <row r="161" spans="1:4">
       <c r="A161" t="s">
         <v>2525</v>
       </c>
@@ -27788,7 +27787,7 @@
         <v/>
       </c>
     </row>
-    <row r="162" spans="1:4" hidden="1">
+    <row r="162" spans="1:4">
       <c r="A162" t="s">
         <v>2527</v>
       </c>
@@ -27800,7 +27799,7 @@
         <v/>
       </c>
     </row>
-    <row r="163" spans="1:4" hidden="1">
+    <row r="163" spans="1:4">
       <c r="A163" t="s">
         <v>2529</v>
       </c>
@@ -27812,7 +27811,7 @@
         <v/>
       </c>
     </row>
-    <row r="164" spans="1:4" hidden="1">
+    <row r="164" spans="1:4">
       <c r="A164" t="s">
         <v>2531</v>
       </c>
@@ -27824,7 +27823,7 @@
         <v/>
       </c>
     </row>
-    <row r="165" spans="1:4" hidden="1">
+    <row r="165" spans="1:4">
       <c r="A165" t="s">
         <v>2533</v>
       </c>
@@ -27836,7 +27835,7 @@
         <v/>
       </c>
     </row>
-    <row r="166" spans="1:4" hidden="1">
+    <row r="166" spans="1:4">
       <c r="A166" t="s">
         <v>2535</v>
       </c>
@@ -27848,7 +27847,7 @@
         <v/>
       </c>
     </row>
-    <row r="167" spans="1:4" hidden="1">
+    <row r="167" spans="1:4">
       <c r="A167" t="s">
         <v>2537</v>
       </c>
@@ -27860,7 +27859,7 @@
         <v/>
       </c>
     </row>
-    <row r="168" spans="1:4" hidden="1">
+    <row r="168" spans="1:4">
       <c r="A168" t="s">
         <v>2539</v>
       </c>
@@ -27872,7 +27871,7 @@
         <v/>
       </c>
     </row>
-    <row r="169" spans="1:4" hidden="1">
+    <row r="169" spans="1:4">
       <c r="A169" t="s">
         <v>2541</v>
       </c>
@@ -27884,7 +27883,7 @@
         <v/>
       </c>
     </row>
-    <row r="170" spans="1:4" hidden="1">
+    <row r="170" spans="1:4">
       <c r="A170" t="s">
         <v>2543</v>
       </c>
@@ -27896,7 +27895,7 @@
         <v/>
       </c>
     </row>
-    <row r="171" spans="1:4" hidden="1">
+    <row r="171" spans="1:4">
       <c r="A171" t="s">
         <v>2545</v>
       </c>
@@ -27908,7 +27907,7 @@
         <v/>
       </c>
     </row>
-    <row r="172" spans="1:4" hidden="1">
+    <row r="172" spans="1:4">
       <c r="A172" t="s">
         <v>2547</v>
       </c>
@@ -27920,7 +27919,7 @@
         <v/>
       </c>
     </row>
-    <row r="173" spans="1:4" hidden="1">
+    <row r="173" spans="1:4">
       <c r="A173" t="s">
         <v>2549</v>
       </c>
@@ -27932,7 +27931,7 @@
         <v/>
       </c>
     </row>
-    <row r="174" spans="1:4" hidden="1">
+    <row r="174" spans="1:4">
       <c r="A174" t="s">
         <v>2551</v>
       </c>
@@ -27944,7 +27943,7 @@
         <v/>
       </c>
     </row>
-    <row r="175" spans="1:4" hidden="1">
+    <row r="175" spans="1:4">
       <c r="A175" t="s">
         <v>2553</v>
       </c>
@@ -27956,19 +27955,22 @@
         <v/>
       </c>
     </row>
-    <row r="176" spans="1:4" hidden="1">
+    <row r="176" spans="1:4">
       <c r="A176" t="s">
         <v>2555</v>
       </c>
       <c r="B176" t="s">
         <v>2556</v>
       </c>
+      <c r="C176" s="1" t="s">
+        <v>2223</v>
+      </c>
       <c r="D176" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="177" spans="1:4" hidden="1">
+    <row r="177" spans="1:4">
       <c r="A177" t="s">
         <v>2557</v>
       </c>
@@ -28007,7 +28009,7 @@
         <v/>
       </c>
     </row>
-    <row r="180" spans="1:4" hidden="1">
+    <row r="180" spans="1:4">
       <c r="A180" t="s">
         <v>2563</v>
       </c>
@@ -28019,7 +28021,7 @@
         <v/>
       </c>
     </row>
-    <row r="181" spans="1:4" hidden="1">
+    <row r="181" spans="1:4">
       <c r="A181" t="s">
         <v>2565</v>
       </c>
@@ -28031,7 +28033,7 @@
         <v/>
       </c>
     </row>
-    <row r="182" spans="1:4" hidden="1">
+    <row r="182" spans="1:4">
       <c r="A182" t="s">
         <v>2567</v>
       </c>
@@ -28043,7 +28045,7 @@
         <v/>
       </c>
     </row>
-    <row r="183" spans="1:4" hidden="1">
+    <row r="183" spans="1:4">
       <c r="A183" t="s">
         <v>2569</v>
       </c>
@@ -28055,7 +28057,7 @@
         <v/>
       </c>
     </row>
-    <row r="184" spans="1:4" hidden="1">
+    <row r="184" spans="1:4">
       <c r="A184" t="s">
         <v>2571</v>
       </c>
@@ -28067,7 +28069,7 @@
         <v/>
       </c>
     </row>
-    <row r="185" spans="1:4" hidden="1">
+    <row r="185" spans="1:4">
       <c r="A185" t="s">
         <v>2573</v>
       </c>
@@ -28079,7 +28081,7 @@
         <v/>
       </c>
     </row>
-    <row r="186" spans="1:4" hidden="1">
+    <row r="186" spans="1:4">
       <c r="A186" t="s">
         <v>2575</v>
       </c>
@@ -28106,7 +28108,7 @@
         <v/>
       </c>
     </row>
-    <row r="188" spans="1:4" hidden="1">
+    <row r="188" spans="1:4">
       <c r="A188" t="s">
         <v>2579</v>
       </c>
@@ -28193,7 +28195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:4" hidden="1">
+    <row r="194" spans="1:4">
       <c r="A194" t="s">
         <v>2591</v>
       </c>
@@ -28205,7 +28207,7 @@
         <v/>
       </c>
     </row>
-    <row r="195" spans="1:4" hidden="1">
+    <row r="195" spans="1:4">
       <c r="A195" t="s">
         <v>2593</v>
       </c>
@@ -28217,7 +28219,7 @@
         <v/>
       </c>
     </row>
-    <row r="196" spans="1:4" hidden="1">
+    <row r="196" spans="1:4">
       <c r="A196" t="s">
         <v>2214</v>
       </c>
@@ -28229,7 +28231,7 @@
         <v/>
       </c>
     </row>
-    <row r="197" spans="1:4" hidden="1">
+    <row r="197" spans="1:4">
       <c r="A197" t="s">
         <v>2216</v>
       </c>
@@ -28242,13 +28244,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D197" xr:uid="{D3918117-006D-4ADF-8B53-EA27F0E01106}">
-    <filterColumn colId="2">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D197" xr:uid="{D3918117-006D-4ADF-8B53-EA27F0E01106}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>